<commit_message>
Rework freight_network module to prefer composition over inheritance. Rework optimization module to save code moving pieces of code to base class methods.
</commit_message>
<xml_diff>
--- a/reports/freight_network_report.xlsx
+++ b/reports/freight_network_report.xlsx
@@ -15,12 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>current situation</t>
   </si>
   <si>
     <t>derive all to railway</t>
+  </si>
+  <si>
+    <t>derive all to railway but some links and ods</t>
+  </si>
+  <si>
+    <t>derive all to roadway</t>
   </si>
   <si>
     <t>Railway</t>
@@ -395,7 +401,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -403,7 +409,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -416,184 +422,316 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01770963192793012</v>
+        <v>0.01673288945463422</v>
       </c>
       <c r="C3" t="n">
         <v>0.06</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01830341875674674</v>
+        <v>0.01682407363005063</v>
       </c>
       <c r="E3" t="n">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="n">
+        <v>0.01535146078091466</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02764712642221689</v>
+        <v>0.02105120441005193</v>
       </c>
       <c r="C4" t="n">
-        <v>0.005669303739094337</v>
+        <v>0.003042183011010634</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01799711037527476</v>
+        <v>0.01355968717530345</v>
       </c>
       <c r="E4" t="n">
-        <v>0.007363221094500188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.003985364225231654</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01339186044923087</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.003980381563050282</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.002852436673808958</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>0.007764478229941269</v>
+        <v>0.006639523351356369</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0050671637145318</v>
+        <v>0.004468860388709386</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="n">
+        <v>0.00429881569672497</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05312123658008829</v>
+        <v>0.04442361721604252</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06566930373909434</v>
+        <v>0.06304218301101064</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0413676928465533</v>
+        <v>0.03485262119406347</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06736322109450019</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.06398536422523166</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.03304213692687051</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.06398038156305029</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.06285243667380896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="n"/>
       <c r="B7" t="n"/>
       <c r="C7" t="n"/>
       <c r="D7" t="n"/>
-      <c r="E7" t="s"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" t="n"/>
+      <c r="F7" t="n"/>
+      <c r="G7" t="n"/>
+      <c r="H7" t="n"/>
+      <c r="I7" t="s"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>25786575.15241584</v>
+        <v>51573150.30483168</v>
       </c>
       <c r="C8" t="n">
-        <v>408913543</v>
+        <v>817827086</v>
       </c>
       <c r="D8" t="n">
-        <v>84743078.30261242</v>
+        <v>172086384.8436974</v>
       </c>
       <c r="E8" t="n">
-        <v>349957039.8498033</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>697313851.4611343</v>
+      </c>
+      <c r="F8" t="n">
+        <v>172412121.4240469</v>
+      </c>
+      <c r="G8" t="n">
+        <v>696988114.8807843</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>869400236.3048313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>11527854554.62704</v>
+        <v>23055709109.25407</v>
       </c>
       <c r="C9" t="n">
-        <v>121914454994.2</v>
+        <v>243828909988.4</v>
       </c>
       <c r="D9" t="n">
-        <v>43496291142.88696</v>
+        <v>88991953205.37643</v>
       </c>
       <c r="E9" t="n">
-        <v>91704327895.44424</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>181584220755.1963</v>
+      </c>
+      <c r="F9" t="n">
+        <v>89287153894.44788</v>
+      </c>
+      <c r="G9" t="n">
+        <v>181940718816.9216</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>265349447068.8743</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>612373889.057191</v>
+        <v>1024217996.113927</v>
       </c>
       <c r="C10" t="n">
-        <v>8006037375.200266</v>
+        <v>15371506766.86395</v>
       </c>
       <c r="D10" t="n">
-        <v>1799341211.963205</v>
+        <v>3101602834.386807</v>
       </c>
       <c r="E10" t="n">
-        <v>6177498915.343351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>11618732502.57611</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2950238364.790906</v>
+      </c>
+      <c r="G10" t="n">
+        <v>11640636611.76229</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>16677859318.32664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="n"/>
       <c r="B11" t="n"/>
       <c r="C11" t="n"/>
       <c r="D11" t="n"/>
-      <c r="E11" t="s"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" t="n"/>
+      <c r="F11" t="n"/>
+      <c r="G11" t="n"/>
+      <c r="H11" t="n"/>
+      <c r="I11" t="s"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="n"/>
       <c r="B12" t="n"/>
       <c r="C12" t="n"/>
       <c r="D12" t="n"/>
-      <c r="E12" t="s"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12" t="n"/>
+      <c r="F12" t="n"/>
+      <c r="G12" t="n"/>
+      <c r="H12" t="n"/>
+      <c r="I12" t="s"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="n"/>
       <c r="B13" t="n"/>
       <c r="C13" t="n"/>
       <c r="D13" t="n"/>
-      <c r="E13" t="s"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" t="n"/>
+      <c r="F13" t="n"/>
+      <c r="G13" t="n"/>
+      <c r="H13" t="n"/>
+      <c r="I13" t="s"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>29.75022641440922</v>
+        <v>35.15135397340254</v>
       </c>
       <c r="C14" t="n"/>
       <c r="D14" t="n">
-        <v>25.62838989260253</v>
+        <v>29.54178128674073</v>
       </c>
       <c r="E14" t="n"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="n">
+        <v>35.34413777669615</v>
+      </c>
+      <c r="G14" t="n"/>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
         <v>447.0486866320841</v>
@@ -602,15 +740,27 @@
         <v>298.1423752800479</v>
       </c>
       <c r="D15" t="n">
-        <v>513.2724939205575</v>
+        <v>517.1353520280295</v>
       </c>
       <c r="E15" t="n">
-        <v>262.0445296222715</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>260.4052972341066</v>
+      </c>
+      <c r="F15" t="n">
+        <v>517.8705137259259</v>
+      </c>
+      <c r="G15" t="n">
+        <v>261.0384810479035</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>305.209771044779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="n">
         <v>17332.3</v>
@@ -619,27 +769,51 @@
         <v>32932.8</v>
       </c>
       <c r="D16" t="n">
-        <v>20883.3</v>
+        <v>21041.3</v>
       </c>
       <c r="E16" t="n">
         <v>32932.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="n">
+        <v>20310.3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>32932.8</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>33460.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>665108.1826778348</v>
+        <v>1330216.36535567</v>
       </c>
       <c r="C17" t="n">
-        <v>3701915.870931107</v>
+        <v>7403831.741862214</v>
       </c>
       <c r="D17" t="n">
-        <v>2082826.523724074</v>
+        <v>4229394.248709748</v>
       </c>
       <c r="E17" t="n">
-        <v>2784589.463861082</v>
+        <v>5513780.205606456</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4396151.405663524</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5524605.220841277</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7930158.486015704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace many get methods with @property decorators.
</commit_message>
<xml_diff>
--- a/reports/freight_network_report.xlsx
+++ b/reports/freight_network_report.xlsx
@@ -15,18 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>current situation</t>
   </si>
   <si>
     <t>derive all to railway</t>
-  </si>
-  <si>
-    <t>derive all to railway but some links and ods</t>
-  </si>
-  <si>
-    <t>derive all to roadway</t>
   </si>
   <si>
     <t>Railway</t>
@@ -401,7 +395,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,7 +403,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -422,316 +416,184 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
       <c r="B3" t="n">
-        <v>0.01673288945463422</v>
+        <v>0.01770963192793012</v>
       </c>
       <c r="C3" t="n">
         <v>0.06</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01682407363005063</v>
+        <v>0.01830341875674674</v>
       </c>
       <c r="E3" t="n">
         <v>0.06</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.01535146078091466</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02105120441005193</v>
+        <v>0.02764712642221689</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003042183011010634</v>
+        <v>0.005669303739094337</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01355968717530345</v>
+        <v>0.01799711037527476</v>
       </c>
       <c r="E4" t="n">
-        <v>0.003985364225231654</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.01339186044923087</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.003980381563050282</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.002852436673808958</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.007363221094500188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.006639523351356369</v>
+        <v>0.007764478229941269</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.004468860388709386</v>
+        <v>0.0050671637145318</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.00429881569672497</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.04442361721604252</v>
+        <v>0.05312123658008829</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06304218301101064</v>
+        <v>0.06566930373909434</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03485262119406347</v>
+        <v>0.0413676928465533</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06398536422523166</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.03304213692687051</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.06398038156305029</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.06285243667380896</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0.06736322109450019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="n"/>
       <c r="B7" t="n"/>
       <c r="C7" t="n"/>
       <c r="D7" t="n"/>
-      <c r="E7" t="n"/>
-      <c r="F7" t="n"/>
-      <c r="G7" t="n"/>
-      <c r="H7" t="n"/>
-      <c r="I7" t="s"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="E7" t="s"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>25786575.15241584</v>
+      </c>
+      <c r="C8" t="n">
+        <v>408913543</v>
+      </c>
+      <c r="D8" t="n">
+        <v>84743078.30261242</v>
+      </c>
+      <c r="E8" t="n">
+        <v>349957039.8498033</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>11527854554.62704</v>
+      </c>
+      <c r="C9" t="n">
+        <v>121914454994.2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>43496291142.88696</v>
+      </c>
+      <c r="E9" t="n">
+        <v>91704327895.44424</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>51573150.30483168</v>
-      </c>
-      <c r="C8" t="n">
-        <v>817827086</v>
-      </c>
-      <c r="D8" t="n">
-        <v>172086384.8436974</v>
-      </c>
-      <c r="E8" t="n">
-        <v>697313851.4611343</v>
-      </c>
-      <c r="F8" t="n">
-        <v>172412121.4240469</v>
-      </c>
-      <c r="G8" t="n">
-        <v>696988114.8807843</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>869400236.3048313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="n">
-        <v>23055709109.25407</v>
-      </c>
-      <c r="C9" t="n">
-        <v>243828909988.4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>88991953205.37643</v>
-      </c>
-      <c r="E9" t="n">
-        <v>181584220755.1963</v>
-      </c>
-      <c r="F9" t="n">
-        <v>89287153894.44788</v>
-      </c>
-      <c r="G9" t="n">
-        <v>181940718816.9216</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>265349447068.8743</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
       <c r="B10" t="n">
-        <v>1024217996.113927</v>
+        <v>612373889.057191</v>
       </c>
       <c r="C10" t="n">
-        <v>15371506766.86395</v>
+        <v>8006037375.200266</v>
       </c>
       <c r="D10" t="n">
-        <v>3101602834.386807</v>
+        <v>1799341211.963205</v>
       </c>
       <c r="E10" t="n">
-        <v>11618732502.57611</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2950238364.790906</v>
-      </c>
-      <c r="G10" t="n">
-        <v>11640636611.76229</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>16677859318.32664</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>6177498915.343351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="n"/>
       <c r="B11" t="n"/>
       <c r="C11" t="n"/>
       <c r="D11" t="n"/>
-      <c r="E11" t="n"/>
-      <c r="F11" t="n"/>
-      <c r="G11" t="n"/>
-      <c r="H11" t="n"/>
-      <c r="I11" t="s"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="E11" t="s"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="n"/>
       <c r="B12" t="n"/>
       <c r="C12" t="n"/>
       <c r="D12" t="n"/>
-      <c r="E12" t="n"/>
-      <c r="F12" t="n"/>
-      <c r="G12" t="n"/>
-      <c r="H12" t="n"/>
-      <c r="I12" t="s"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="E12" t="s"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="n"/>
       <c r="B13" t="n"/>
       <c r="C13" t="n"/>
       <c r="D13" t="n"/>
-      <c r="E13" t="n"/>
-      <c r="F13" t="n"/>
-      <c r="G13" t="n"/>
-      <c r="H13" t="n"/>
-      <c r="I13" t="s"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="E13" t="s"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="n">
-        <v>35.15135397340254</v>
+        <v>29.75022641440922</v>
       </c>
       <c r="C14" t="n"/>
       <c r="D14" t="n">
-        <v>29.54178128674073</v>
+        <v>25.62838989260253</v>
       </c>
       <c r="E14" t="n"/>
-      <c r="F14" t="n">
-        <v>35.34413777669615</v>
-      </c>
-      <c r="G14" t="n"/>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="n">
         <v>447.0486866320841</v>
@@ -740,27 +602,15 @@
         <v>298.1423752800479</v>
       </c>
       <c r="D15" t="n">
-        <v>517.1353520280295</v>
+        <v>513.2724939205575</v>
       </c>
       <c r="E15" t="n">
-        <v>260.4052972341066</v>
-      </c>
-      <c r="F15" t="n">
-        <v>517.8705137259259</v>
-      </c>
-      <c r="G15" t="n">
-        <v>261.0384810479035</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>305.209771044779</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>262.0445296222715</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="n">
         <v>17332.3</v>
@@ -769,51 +619,27 @@
         <v>32932.8</v>
       </c>
       <c r="D16" t="n">
-        <v>21041.3</v>
+        <v>20883.3</v>
       </c>
       <c r="E16" t="n">
         <v>32932.8</v>
       </c>
-      <c r="F16" t="n">
-        <v>20310.3</v>
-      </c>
-      <c r="G16" t="n">
-        <v>32932.8</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>33460.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n">
-        <v>1330216.36535567</v>
+        <v>665108.1826778348</v>
       </c>
       <c r="C17" t="n">
-        <v>7403831.741862214</v>
+        <v>3701915.870931107</v>
       </c>
       <c r="D17" t="n">
-        <v>4229394.248709748</v>
+        <v>2082826.523724074</v>
       </c>
       <c r="E17" t="n">
-        <v>5513780.205606456</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4396151.405663524</v>
-      </c>
-      <c r="G17" t="n">
-        <v>5524605.220841277</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>7930158.486015704</v>
+        <v>2784589.463861082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rework find_paths module, taking out methods to find shortest paths and moving them to classes in path_finder module.
</commit_message>
<xml_diff>
--- a/reports/freight_network_report.xlsx
+++ b/reports/freight_network_report.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="global_results" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="270" yWindow="525" windowWidth="19815" windowHeight="7110"/>
+  </bookViews>
+  <sheets>
+    <sheet name="global_results" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="145621"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>current situation</t>
+  </si>
+  <si>
+    <t>derive all to railway</t>
+  </si>
+  <si>
+    <t>derive all to railway but some links and ods</t>
+  </si>
+  <si>
+    <t>derive all to roadway</t>
   </si>
   <si>
     <t>Railway</t>
@@ -62,12 +70,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,21 +109,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -179,6 +203,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -213,6 +238,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,174 +414,407 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.01812407162286442</v>
-      </c>
-      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1.8124071622864418E-2</v>
+      </c>
+      <c r="C3">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>1.952133914878576E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.06</v>
+      </c>
+      <c r="F3">
+        <v>1.602310611549345E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.06</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0276558058426621</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.005669303739094337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2.7655805842662098E-2</v>
+      </c>
+      <c r="C4">
+        <v>5.6693037390943366E-3</v>
+      </c>
+      <c r="D4">
+        <v>1.8080383597712441E-2</v>
+      </c>
+      <c r="E4">
+        <v>7.3812729768914552E-3</v>
+      </c>
+      <c r="F4">
+        <v>1.7646726287315138E-2</v>
+      </c>
+      <c r="G4">
+        <v>7.1517517208234543E-3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>5.3068649287889196E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.008085601613934908</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>8.0856016139349077E-3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>5.2204598855487916E-3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4.8294846399924898E-3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.05386547907946142</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.06566930373909434</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="n"/>
-      <c r="B7" t="n"/>
-      <c r="C7" t="s"/>
-    </row>
-    <row r="8" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>5.3865479079461417E-2</v>
+      </c>
+      <c r="C6">
+        <v>6.566930373909434E-2</v>
+      </c>
+      <c r="D6">
+        <v>4.2822182632046991E-2</v>
+      </c>
+      <c r="E6">
+        <v>6.7381272976891463E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.849931704280108E-2</v>
+      </c>
+      <c r="G6">
+        <v>6.7151751720823466E-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>6.5306864928788927E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>26412937.54733584</v>
-      </c>
-      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>26412937.547335841</v>
+      </c>
+      <c r="C8">
         <v>408913543</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>86037254.840407237</v>
+      </c>
+      <c r="E8">
+        <v>349289225.70692861</v>
+      </c>
+      <c r="F8">
+        <v>79252763.675825059</v>
+      </c>
+      <c r="G8">
+        <v>356073716.87151092</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>435326480.54733562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>11260463543.3734</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>121914454994.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>43286548839.377899</v>
+      </c>
+      <c r="E9">
+        <v>91452440432.656128</v>
+      </c>
+      <c r="F9">
+        <v>39538997295.480202</v>
+      </c>
+      <c r="G9">
+        <v>94971794722.088486</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>132447799070.795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>606550263.4206179</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8006037375.200266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="n"/>
-      <c r="B11" t="n"/>
-      <c r="C11" t="s"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="n"/>
-      <c r="B12" t="n"/>
-      <c r="C12" t="s"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="n"/>
-      <c r="B13" t="n"/>
-      <c r="C13" t="s"/>
-    </row>
-    <row r="14" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>606550263.42061794</v>
+      </c>
+      <c r="C10">
+        <v>8006037375.2002659</v>
+      </c>
+      <c r="D10">
+        <v>1853624499.910862</v>
+      </c>
+      <c r="E10">
+        <v>6162181853.1957083</v>
+      </c>
+      <c r="F10">
+        <v>1522224392.433147</v>
+      </c>
+      <c r="G10">
+        <v>6377522379.6586981</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8649750524.0317822</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>SUM(B10:C10)</f>
+        <v>8612587638.6208839</v>
+      </c>
+      <c r="E11">
+        <f>SUM(D10:E10)</f>
+        <v>8015806353.1065702</v>
+      </c>
+      <c r="G11">
+        <f>SUM(F10:G10)</f>
+        <v>7899746772.0918446</v>
+      </c>
+      <c r="I11">
+        <f>SUM(H10:I10)</f>
+        <v>8649750524.0317822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <f>G11/C11-1</f>
+        <v>-8.2767328059745071E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="n">
-        <v>30.55844680252241</v>
-      </c>
-      <c r="C14" t="n"/>
-    </row>
-    <row r="15" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>30.558446802522411</v>
+      </c>
+      <c r="D14">
+        <v>18.822191112203921</v>
+      </c>
+      <c r="F14">
+        <v>31.805754815980279</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="n">
-        <v>426.3237863336103</v>
-      </c>
-      <c r="C15" t="n">
-        <v>298.1423752800479</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>426.32378633361031</v>
+      </c>
+      <c r="C15">
+        <v>298.14237528004787</v>
+      </c>
+      <c r="D15">
+        <v>503.11401636036919</v>
+      </c>
+      <c r="E15">
+        <v>261.82439566398023</v>
+      </c>
+      <c r="F15">
+        <v>498.89739438248779</v>
+      </c>
+      <c r="G15">
+        <v>266.71947471022992</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>304.24935074996688</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>17278.3</v>
       </c>
-      <c r="C16" t="n">
-        <v>32932.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16">
+        <v>32932.800000000003</v>
+      </c>
+      <c r="D16">
+        <v>21024.3</v>
+      </c>
+      <c r="E16">
+        <v>32932.800000000003</v>
+      </c>
+      <c r="F16">
+        <v>18525.3</v>
+      </c>
+      <c r="G16">
+        <v>32932.800000000003</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>33290.800000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="n">
-        <v>651711.310914465</v>
-      </c>
-      <c r="C17" t="n">
-        <v>3701915.870931107</v>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>651711.31091446499</v>
+      </c>
+      <c r="C17">
+        <v>3701915.8709311071</v>
+      </c>
+      <c r="D17">
+        <v>2058881.810066347</v>
+      </c>
+      <c r="E17">
+        <v>2776940.9352577408</v>
+      </c>
+      <c r="F17">
+        <v>2134324.2644103039</v>
+      </c>
+      <c r="G17">
+        <v>2883805.6503573479</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>3978510.5515876738</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add costing scenarios with link restrictions to the main method.
</commit_message>
<xml_diff>
--- a/reports/freight_network_report.xlsx
+++ b/reports/freight_network_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>current situation</t>
   </si>
@@ -23,7 +23,22 @@
     <t>derive all to railway</t>
   </si>
   <si>
+    <t>derive all to railway but some links and ods</t>
+  </si>
+  <si>
     <t>derive all to roadway</t>
+  </si>
+  <si>
+    <t>current situation RESTR</t>
+  </si>
+  <si>
+    <t>derive all to railway RESTR</t>
+  </si>
+  <si>
+    <t>derive all to railway but some links and ods RESTR</t>
+  </si>
+  <si>
+    <t>derive all to roadway RESTR</t>
   </si>
   <si>
     <t>Railway</t>
@@ -398,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:17">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -425,307 +440,727 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01758013451409797</v>
+        <v>0.0181173249816075</v>
       </c>
       <c r="C3" t="n">
         <v>0.06</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01818591039112635</v>
+        <v>0.01851074119649518</v>
       </c>
       <c r="E3" t="n">
         <v>0.06</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.01592112165402621</v>
       </c>
       <c r="G3" t="n">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.01758013451409797</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.01818591039112635</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.01583805738890978</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02640836961971154</v>
+        <v>0.0276558058426621</v>
       </c>
       <c r="C4" t="n">
         <v>0.005669303739094337</v>
       </c>
       <c r="D4" t="n">
+        <v>0.01808038359771244</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.007381272976891455</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01768648366784235</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.00718892366363924</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.00530686492878892</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.02640836961971154</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.005669303739094337</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.01707688772092151</v>
       </c>
-      <c r="E4" t="n">
+      <c r="M4" t="n">
         <v>0.007230714419536676</v>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="N4" t="n">
+        <v>0.01681874935807088</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.007115413932215001</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0.005290409086069071</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
+        <v>0.008085601613934908</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.005220459885548792</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.004756281663981725</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.007424250951861848</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.004901654290261846</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.004543205637767161</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05141275508567135</v>
+        <v>0.05385873243820451</v>
       </c>
       <c r="C6" t="n">
         <v>0.06566930373909434</v>
       </c>
       <c r="D6" t="n">
+        <v>0.04181158467975642</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.06738127297689146</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.03836388698585028</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.06718892366363924</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.06530686492878893</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.05141275508567135</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.06566930373909434</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.04016445240230972</v>
       </c>
-      <c r="E6" t="n">
+      <c r="M6" t="n">
         <v>0.06723071441953668</v>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="N6" t="n">
+        <v>0.03720001238474781</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.06711541393221501</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>0.06529040908606908</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:17">
       <c r="A7" t="n"/>
       <c r="B7" t="n"/>
       <c r="C7" t="n"/>
       <c r="D7" t="n"/>
       <c r="E7" t="n"/>
       <c r="F7" t="n"/>
-      <c r="G7" t="s"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" t="n"/>
+      <c r="H7" t="n"/>
+      <c r="I7" t="n"/>
+      <c r="J7" t="n"/>
+      <c r="K7" t="n"/>
+      <c r="L7" t="n"/>
+      <c r="M7" t="n"/>
+      <c r="N7" t="n"/>
+      <c r="O7" t="n"/>
+      <c r="P7" t="n"/>
+      <c r="Q7" t="s"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>26004837.54733584</v>
+        <v>26412937.54733584</v>
       </c>
       <c r="C8" t="n">
         <v>408913543</v>
       </c>
       <c r="D8" t="n">
+        <v>86037254.84040724</v>
+      </c>
+      <c r="E8" t="n">
+        <v>349289225.7069286</v>
+      </c>
+      <c r="F8" t="n">
+        <v>79909788.30960095</v>
+      </c>
+      <c r="G8" t="n">
+        <v>355416692.2377349</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>435326480.5473356</v>
+      </c>
+      <c r="J8" t="n">
+        <v>26004837.54733584</v>
+      </c>
+      <c r="K8" t="n">
+        <v>408913543</v>
+      </c>
+      <c r="L8" t="n">
         <v>80813879.38183784</v>
       </c>
-      <c r="E8" t="n">
+      <c r="M8" t="n">
         <v>354104501.1654981</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="N8" t="n">
+        <v>77562092.98920457</v>
+      </c>
+      <c r="O8" t="n">
+        <v>357356287.5581313</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
         <v>434918380.5473356</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>11573679240.83252</v>
+        <v>11260463543.3734</v>
       </c>
       <c r="C9" t="n">
         <v>121914454994.2</v>
       </c>
       <c r="D9" t="n">
+        <v>43286548839.3779</v>
+      </c>
+      <c r="E9" t="n">
+        <v>91452440432.65613</v>
+      </c>
+      <c r="F9" t="n">
+        <v>40249299093.38931</v>
+      </c>
+      <c r="G9" t="n">
+        <v>94357254846.23744</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>132447799070.795</v>
+      </c>
+      <c r="J9" t="n">
+        <v>11573679240.83252</v>
+      </c>
+      <c r="K9" t="n">
+        <v>121914454994.2</v>
+      </c>
+      <c r="L9" t="n">
         <v>41394399934.05531</v>
       </c>
-      <c r="E9" t="n">
+      <c r="M9" t="n">
         <v>93669995343.11043</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="N9" t="n">
+        <v>39643175183.15067</v>
+      </c>
+      <c r="O9" t="n">
+        <v>95438029466.20343</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
         <v>132282464010.795</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>595034736.2490411</v>
+        <v>606474293.1127042</v>
       </c>
       <c r="C10" t="n">
         <v>8006037375.200266</v>
       </c>
       <c r="D10" t="n">
+        <v>1809879202.292061</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6162181853.195708</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1544119561.678474</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6339762392.974401</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8649750524.031782</v>
+      </c>
+      <c r="J10" t="n">
+        <v>595034736.2490411</v>
+      </c>
+      <c r="K10" t="n">
+        <v>8006037375.200266</v>
+      </c>
+      <c r="L10" t="n">
         <v>1662583405.873537</v>
       </c>
-      <c r="E10" t="n">
+      <c r="M10" t="n">
         <v>6297500706.591988</v>
       </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
+      <c r="N10" t="n">
+        <v>1474726607.783932</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6405362852.499177</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
         <v>8636776190.178013</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:17">
       <c r="A11" t="n"/>
       <c r="B11" t="n"/>
       <c r="C11" t="n"/>
       <c r="D11" t="n"/>
       <c r="E11" t="n"/>
       <c r="F11" t="n"/>
-      <c r="G11" t="s"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" t="n"/>
+      <c r="H11" t="n"/>
+      <c r="I11" t="n"/>
+      <c r="J11" t="n"/>
+      <c r="K11" t="n"/>
+      <c r="L11" t="n"/>
+      <c r="M11" t="n"/>
+      <c r="N11" t="n"/>
+      <c r="O11" t="n"/>
+      <c r="P11" t="n"/>
+      <c r="Q11" t="s"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="n"/>
       <c r="B12" t="n"/>
       <c r="C12" t="n"/>
       <c r="D12" t="n"/>
       <c r="E12" t="n"/>
       <c r="F12" t="n"/>
-      <c r="G12" t="s"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" t="n"/>
+      <c r="H12" t="n"/>
+      <c r="I12" t="n"/>
+      <c r="J12" t="n"/>
+      <c r="K12" t="n"/>
+      <c r="L12" t="n"/>
+      <c r="M12" t="n"/>
+      <c r="N12" t="n"/>
+      <c r="O12" t="n"/>
+      <c r="P12" t="n"/>
+      <c r="Q12" t="s"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="n"/>
       <c r="B13" t="n"/>
       <c r="C13" t="n"/>
       <c r="D13" t="n"/>
       <c r="E13" t="n"/>
       <c r="F13" t="n"/>
-      <c r="G13" t="s"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" t="n"/>
+      <c r="H13" t="n"/>
+      <c r="I13" t="n"/>
+      <c r="J13" t="n"/>
+      <c r="K13" t="n"/>
+      <c r="L13" t="n"/>
+      <c r="M13" t="n"/>
+      <c r="N13" t="n"/>
+      <c r="O13" t="n"/>
+      <c r="P13" t="n"/>
+      <c r="Q13" t="s"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>30.72693811630958</v>
+        <v>30.80917784567212</v>
       </c>
       <c r="C14" t="n"/>
       <c r="D14" t="n">
-        <v>26.29589173559053</v>
+        <v>25.95704633652343</v>
       </c>
       <c r="E14" t="n"/>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>34.31212090664163</v>
       </c>
       <c r="G14" t="n"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n"/>
+      <c r="J14" t="n">
+        <v>30.72693811630958</v>
+      </c>
+      <c r="K14" t="n"/>
+      <c r="L14" t="n">
+        <v>26.29589173559053</v>
+      </c>
+      <c r="M14" t="n"/>
+      <c r="N14" t="n">
+        <v>33.81121913786672</v>
+      </c>
+      <c r="O14" t="n"/>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>445.0587018575022</v>
+        <v>426.3237863336103</v>
       </c>
       <c r="C15" t="n">
         <v>298.1423752800479</v>
       </c>
       <c r="D15" t="n">
+        <v>503.1140163603692</v>
+      </c>
+      <c r="E15" t="n">
+        <v>261.8243956639802</v>
+      </c>
+      <c r="F15" t="n">
+        <v>503.6842162245281</v>
+      </c>
+      <c r="G15" t="n">
+        <v>265.483464640211</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>304.2493507499669</v>
+      </c>
+      <c r="J15" t="n">
+        <v>445.0587018575022</v>
+      </c>
+      <c r="K15" t="n">
+        <v>298.1423752800479</v>
+      </c>
+      <c r="L15" t="n">
         <v>512.2189437097893</v>
       </c>
-      <c r="E15" t="n">
+      <c r="M15" t="n">
         <v>264.5264181472006</v>
       </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
+      <c r="N15" t="n">
+        <v>511.1153355372756</v>
+      </c>
+      <c r="O15" t="n">
+        <v>267.0668819579073</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
         <v>304.154687241133</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>15713.3</v>
+        <v>17278.3</v>
       </c>
       <c r="C16" t="n">
         <v>32932.8</v>
       </c>
       <c r="D16" t="n">
-        <v>17456.3</v>
+        <v>21024.3</v>
       </c>
       <c r="E16" t="n">
         <v>32932.8</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>18865.3</v>
       </c>
       <c r="G16" t="n">
+        <v>32932.8</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>33290.8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>15713.3</v>
+      </c>
+      <c r="K16" t="n">
+        <v>32932.8</v>
+      </c>
+      <c r="L16" t="n">
+        <v>17456.3</v>
+      </c>
+      <c r="M16" t="n">
+        <v>32932.8</v>
+      </c>
+      <c r="N16" t="n">
+        <v>16511.3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>32932.8</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
         <v>33091.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>736553.0627450963</v>
+        <v>651711.310914465</v>
       </c>
       <c r="C17" t="n">
         <v>3701915.870931107</v>
       </c>
       <c r="D17" t="n">
+        <v>2058881.810066347</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2776940.935257741</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2133509.623138212</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2865145.230476529</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3978510.551587674</v>
+      </c>
+      <c r="J17" t="n">
+        <v>736553.0627450963</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3701915.870931107</v>
+      </c>
+      <c r="L17" t="n">
         <v>2371315.79624865</v>
       </c>
-      <c r="E17" t="n">
+      <c r="M17" t="n">
         <v>2844276.688988195</v>
       </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
+      <c r="N17" t="n">
+        <v>2400972.375473201</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2897962.805051603</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
         <v>3997439.365969664</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rail pathless od pairs are now derived to roadway network during FreightNetwork construction.
</commit_message>
<xml_diff>
--- a/reports/freight_network_report.xlsx
+++ b/reports/freight_network_report.xlsx
@@ -540,37 +540,37 @@
         <v>0.02807412015241508</v>
       </c>
       <c r="C4" t="n">
-        <v>0.005669303739094337</v>
+        <v>0.005665227045420121</v>
       </c>
       <c r="D4" t="n">
         <v>0.01773502879962139</v>
       </c>
       <c r="E4" t="n">
-        <v>0.007477675086999053</v>
+        <v>0.007470363524626595</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005366911912577466</v>
+        <v>0.005363387304790163</v>
       </c>
       <c r="H4" t="n">
         <v>0.0268281070608837</v>
       </c>
       <c r="I4" t="n">
-        <v>0.005669303739094337</v>
+        <v>0.005682562833820645</v>
       </c>
       <c r="J4" t="n">
         <v>0.01686467141078661</v>
       </c>
       <c r="K4" t="n">
-        <v>0.007309247669765462</v>
+        <v>0.007322221694108118</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.005350617674784681</v>
+        <v>0.005363387304790163</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -622,37 +622,37 @@
         <v>0.05720460052473796</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06566930373909434</v>
+        <v>0.06566522704542013</v>
       </c>
       <c r="D6" t="n">
         <v>0.04055830460926885</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06747767508699906</v>
+        <v>0.0674703635246266</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.06536691191257747</v>
+        <v>0.06536338730479017</v>
       </c>
       <c r="H6" t="n">
         <v>0.05474478824188233</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06566930373909434</v>
+        <v>0.06568256283382065</v>
       </c>
       <c r="J6" t="n">
         <v>0.03916238099797786</v>
       </c>
       <c r="K6" t="n">
-        <v>0.06730924766976547</v>
+        <v>0.06732222169410812</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.06535061767478469</v>
+        <v>0.06536338730479017</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -678,37 +678,37 @@
         <v>30282900.71486275</v>
       </c>
       <c r="C8" t="n">
-        <v>408913543</v>
+        <v>409093579.8324731</v>
       </c>
       <c r="D8" t="n">
         <v>96431061.77181628</v>
       </c>
       <c r="E8" t="n">
-        <v>342765381.9430466</v>
+        <v>342945418.7755197</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>439196443.7148625</v>
+        <v>439376480.5473356</v>
       </c>
       <c r="H8" t="n">
         <v>29874800.71486275</v>
       </c>
       <c r="I8" t="n">
-        <v>408913543</v>
+        <v>409501679.8324731</v>
       </c>
       <c r="J8" t="n">
         <v>90369755.99866468</v>
       </c>
       <c r="K8" t="n">
-        <v>348418587.716198</v>
+        <v>349006724.5486711</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>438788343.7148625</v>
+        <v>439376480.5473356</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -719,37 +719,37 @@
         <v>11946027185.31634</v>
       </c>
       <c r="C9" t="n">
-        <v>121914454994.2</v>
+        <v>122009715530.0625</v>
       </c>
       <c r="D9" t="n">
         <v>45445633270.44735</v>
       </c>
       <c r="E9" t="n">
-        <v>90223399388.77956</v>
+        <v>90318659924.64212</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>133150478534.9324</v>
+        <v>133245739070.795</v>
       </c>
       <c r="H9" t="n">
         <v>12259242882.77546</v>
       </c>
       <c r="I9" t="n">
-        <v>121914454994.2</v>
+        <v>122175050590.0625</v>
       </c>
       <c r="J9" t="n">
         <v>43343266358.83762</v>
       </c>
       <c r="K9" t="n">
-        <v>92638982380.36638</v>
+        <v>92899577976.22893</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>132985143474.9324</v>
+        <v>133245739070.795</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -760,37 +760,37 @@
         <v>683367712.9936808</v>
       </c>
       <c r="C10" t="n">
-        <v>8006037375.200266</v>
+        <v>8011795672.02868</v>
       </c>
       <c r="D10" t="n">
         <v>1843197837.343926</v>
       </c>
       <c r="E10" t="n">
-        <v>6088065229.200617</v>
+        <v>6093832818.172728</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>8703635601.510464</v>
+        <v>8709392849.597383</v>
       </c>
       <c r="H10" t="n">
         <v>671129655.6233457</v>
       </c>
       <c r="I10" t="n">
-        <v>8006037375.200266</v>
+        <v>8024770437.107</v>
       </c>
       <c r="J10" t="n">
         <v>1697425510.841635</v>
       </c>
       <c r="K10" t="n">
-        <v>6235460208.91512</v>
+        <v>6254205983.804768</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>8690661267.656694</v>
+        <v>8709392849.597383</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -875,37 +875,37 @@
         <v>394.4809414988857</v>
       </c>
       <c r="C15" t="n">
-        <v>298.1423752800479</v>
+        <v>298.2440242157465</v>
       </c>
       <c r="D15" t="n">
         <v>471.2758776625817</v>
       </c>
       <c r="E15" t="n">
-        <v>263.2220292414796</v>
+        <v>263.3616166885192</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>303.1683895450143</v>
+        <v>303.2609731517932</v>
       </c>
       <c r="H15" t="n">
         <v>410.3539635220554</v>
       </c>
       <c r="I15" t="n">
-        <v>298.1423752800479</v>
+        <v>298.3505480125119</v>
       </c>
       <c r="J15" t="n">
         <v>479.6213719939452</v>
       </c>
       <c r="K15" t="n">
-        <v>265.8841567196318</v>
+        <v>266.1827736882861</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>303.0735555759203</v>
+        <v>303.2609731517932</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -934,19 +934,19 @@
         <v>17221.3</v>
       </c>
       <c r="I16" t="n">
-        <v>32932.8</v>
+        <v>33131.8</v>
       </c>
       <c r="J16" t="n">
         <v>17440.3</v>
       </c>
       <c r="K16" t="n">
-        <v>32932.8</v>
+        <v>33131.8</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>33712.8</v>
+        <v>33911.8</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -957,37 +957,37 @@
         <v>619019.6641837019</v>
       </c>
       <c r="C17" t="n">
-        <v>3701915.870931107</v>
+        <v>3704808.444166987</v>
       </c>
       <c r="D17" t="n">
         <v>2189064.381075772</v>
       </c>
       <c r="E17" t="n">
-        <v>2739621.270853968</v>
+        <v>2742513.844089847</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3926376.026484362</v>
+        <v>3929185.094002529</v>
       </c>
       <c r="H17" t="n">
         <v>711865.1253259314</v>
       </c>
       <c r="I17" t="n">
-        <v>3701915.870931107</v>
+        <v>3687546.423377617</v>
       </c>
       <c r="J17" t="n">
         <v>2485236.283712873</v>
       </c>
       <c r="K17" t="n">
-        <v>2812970.120377447</v>
+        <v>2803939.960286761</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>3944648.426560013</v>
+        <v>3929185.094002529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>